<commit_message>
View More page DONE
</commit_message>
<xml_diff>
--- a/EmpUp Payroll.xlsx
+++ b/EmpUp Payroll.xlsx
@@ -1,106 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sap-EmpUp\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
-  </bookViews>
   <sheets>
     <sheet name="Payroll" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Basic</t>
-  </si>
-  <si>
-    <t>Allowance</t>
-  </si>
-  <si>
-    <t>IT</t>
-  </si>
-  <si>
-    <t>StandardDeduction</t>
-  </si>
-  <si>
-    <t>PF</t>
-  </si>
-  <si>
-    <t>payPeriod</t>
-  </si>
-  <si>
-    <t>grossIncome</t>
-  </si>
-  <si>
-    <t>incomeTax</t>
-  </si>
-  <si>
-    <t>netIncome</t>
-  </si>
-  <si>
-    <t>TDS</t>
-  </si>
-  <si>
-    <t>ESI</t>
-  </si>
-  <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>60050</t>
-  </si>
-  <si>
-    <t>15000</t>
-  </si>
-  <si>
-    <t>25000</t>
-  </si>
-  <si>
-    <t>50000</t>
-  </si>
-  <si>
-    <t>01 March - 31 March</t>
-  </si>
-  <si>
-    <t>Ryan</t>
-  </si>
-  <si>
-    <t>120000</t>
-  </si>
-  <si>
-    <t>10000</t>
-  </si>
-  <si>
-    <t>17000</t>
-  </si>
-  <si>
-    <t>Sam</t>
-  </si>
-  <si>
-    <t>20000</t>
-  </si>
-  <si>
-    <t>12000</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -137,14 +50,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -469,72 +374,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Basic</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Allowance</v>
+      </c>
+      <c r="D1" t="str">
+        <v>IT</v>
+      </c>
+      <c r="E1" t="str">
+        <v>StandardDeduction</v>
+      </c>
+      <c r="F1" t="str">
+        <v>PF</v>
+      </c>
+      <c r="G1" t="str">
+        <v>payPeriod</v>
+      </c>
+      <c r="H1" t="str">
+        <v>grossIncome</v>
+      </c>
+      <c r="I1" t="str">
+        <v>incomeTax</v>
+      </c>
+      <c r="J1" t="str">
+        <v>netIncome</v>
+      </c>
+      <c r="K1" t="str">
+        <v>TDS</v>
+      </c>
+      <c r="L1" t="str">
+        <v>ESI</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>David</v>
+      </c>
+      <c r="B2" t="str">
+        <v>60050</v>
+      </c>
+      <c r="C2" t="str">
+        <v>15000</v>
+      </c>
+      <c r="D2" t="str">
+        <v>25000</v>
+      </c>
+      <c r="E2" t="str">
+        <v>50000</v>
       </c>
       <c r="F2">
         <v>9006</v>
       </c>
-      <c r="G2" t="s">
-        <v>17</v>
+      <c r="G2" t="str">
+        <v>01 March - 31 March</v>
       </c>
       <c r="H2">
         <v>75050</v>
@@ -552,27 +456,27 @@
         <v>157.5</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Ryan</v>
+      </c>
+      <c r="B3" t="str">
+        <v>120000</v>
+      </c>
+      <c r="C3" t="str">
+        <v>10000</v>
+      </c>
+      <c r="D3" t="str">
+        <v>17000</v>
+      </c>
+      <c r="E3" t="str">
+        <v>50000</v>
       </c>
       <c r="F3">
         <v>15000</v>
       </c>
-      <c r="G3" t="s">
-        <v>17</v>
+      <c r="G3" t="str">
+        <v>01 March - 31 March</v>
       </c>
       <c r="H3">
         <v>130000</v>
@@ -590,27 +494,27 @@
         <v>157.5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Sam</v>
+      </c>
+      <c r="B4" t="str">
+        <v>20000</v>
+      </c>
+      <c r="C4" t="str">
+        <v>20000</v>
+      </c>
+      <c r="D4" t="str">
+        <v>12000</v>
+      </c>
+      <c r="E4" t="str">
+        <v>50000</v>
       </c>
       <c r="F4">
         <v>2616</v>
       </c>
-      <c r="G4" t="s">
-        <v>17</v>
+      <c r="G4" t="str">
+        <v>01 March - 31 March</v>
       </c>
       <c r="H4">
         <v>40000</v>
@@ -629,9 +533,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:L4" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>